<commit_message>
Redmine ticket #8553 Cal sheets for multiple deployments of CP05MOAS-GL001 modified.
</commit_message>
<xml_diff>
--- a/CP05MOAS-GL001/Omaha_Cal_Info_CP05MOAS-GL001_00001.xlsx
+++ b/CP05MOAS-GL001/Omaha_Cal_Info_CP05MOAS-GL001_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Sheets from -test 2015-08-19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Repaired GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12708" yWindow="48" windowWidth="12516" windowHeight="12336" tabRatio="377" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19836" windowHeight="8052" tabRatio="377" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$79</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$360</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -411,12 +411,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -424,6 +418,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,7 +532,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -573,12 +573,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -586,8 +580,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="12" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="12" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1082,7 +1082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1152,7 +1152,7 @@
       <c r="E2" s="19">
         <v>0.6875</v>
       </c>
-      <c r="F2" s="34">
+      <c r="F2" s="32">
         <v>41918</v>
       </c>
       <c r="G2" s="28" t="s">
@@ -1170,11 +1170,11 @@
       <c r="K2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="32">
+      <c r="L2" s="30">
         <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
         <v>40.109983333333332</v>
       </c>
-      <c r="M2" s="32">
+      <c r="M2" s="30">
         <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
         <v>-70.561199999999999</v>
       </c>
@@ -1189,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1242,7 +1242,7 @@
       <c r="E2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="31">
         <v>0.61</v>
       </c>
       <c r="G2" s="26"/>
@@ -1271,7 +1271,7 @@
       <c r="E3" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="31">
         <v>0.61</v>
       </c>
       <c r="G3" s="26"/>
@@ -1300,7 +1300,7 @@
       <c r="E4" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="31">
         <v>0.61</v>
       </c>
       <c r="G4" s="26"/>
@@ -1329,7 +1329,7 @@
       <c r="E5" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="31">
         <v>0.61</v>
       </c>
       <c r="G5" s="26"/>
@@ -1348,7 +1348,7 @@
       <c r="C6" s="23"/>
       <c r="D6" s="27"/>
       <c r="E6" s="24"/>
-      <c r="F6" s="33"/>
+      <c r="F6" s="31"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -1375,8 +1375,8 @@
       <c r="E7" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="30">
-        <v>117</v>
+      <c r="F7" s="34">
+        <v>124</v>
       </c>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
@@ -1399,7 +1399,7 @@
       <c r="E8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="33">
         <v>700</v>
       </c>
       <c r="G8" s="21"/>
@@ -1423,8 +1423,8 @@
       <c r="E9" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="30">
-        <v>1.08</v>
+      <c r="F9" s="34">
+        <v>1.0760000000000001</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
@@ -1447,7 +1447,7 @@
       <c r="E10" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="33">
         <v>3.9E-2</v>
       </c>
       <c r="G10" s="21"/>
@@ -1461,7 +1461,7 @@
       <c r="C11" s="23"/>
       <c r="D11" s="27"/>
       <c r="E11" s="25"/>
-      <c r="F11" s="31"/>
+      <c r="F11" s="29"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>

</xml_diff>

<commit_message>
Coastal Surface Piercing Profilers
Updated Coastal CSPP ingest and cal sheets
added engineering data streams
Created files where data existed but ingest files were missing
corrected instrument reference designators
</commit_message>
<xml_diff>
--- a/CP05MOAS-GL001/Omaha_Cal_Info_CP05MOAS-GL001_00001.xlsx
+++ b/CP05MOAS-GL001/Omaha_Cal_Info_CP05MOAS-GL001_00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19830" windowHeight="8055" tabRatio="377"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19830" windowHeight="8055" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$79</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$360</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -115,28 +115,28 @@
     <t>Anchor Launch Time</t>
   </si>
   <si>
-    <t>CP05MOAS-GL001-01-ADCPAM000</t>
-  </si>
-  <si>
-    <t>CP05MOAS-GL001-02-FLORTM000</t>
-  </si>
-  <si>
-    <t>CP05MOAS-GL001-03-CTDGVM000</t>
-  </si>
-  <si>
-    <t>CP05MOAS-GL001-04-DOSTAM000</t>
-  </si>
-  <si>
-    <t>CP05MOAS-GL001-05-PARADM000</t>
-  </si>
-  <si>
-    <t>CP05MOAS-GL001-00-ENG000000</t>
-  </si>
-  <si>
     <t>Mooring Serial Number</t>
   </si>
   <si>
-    <t>CP05MOAS-GL001</t>
+    <t>CP05MOAS-GL374</t>
+  </si>
+  <si>
+    <t>CP05MOAS-GL374-01-ADCPAM000</t>
+  </si>
+  <si>
+    <t>CP05MOAS-GL374-02-FLORTM000</t>
+  </si>
+  <si>
+    <t>CP05MOAS-GL374-03-CTDGVM000</t>
+  </si>
+  <si>
+    <t>CP05MOAS-GL374-04-DOSTAM000</t>
+  </si>
+  <si>
+    <t>CP05MOAS-GL374-05-PARADM000</t>
+  </si>
+  <si>
+    <t>CP05MOAS-GL374-00-ENG000000</t>
   </si>
 </sst>
 </file>
@@ -777,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +833,7 @@
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" s="10">
         <v>374</v>
@@ -884,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>11</v>
@@ -923,7 +923,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" s="16">
         <v>374</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="16">
         <v>374</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4" s="16">
         <v>374</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B5" s="16">
         <v>374</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="7" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B7" s="16">
         <v>374</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="8" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="16">
         <v>374</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="9" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="16">
         <v>374</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="10" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" s="16">
         <v>374</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="12" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="16">
         <v>374</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="14" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B14" s="16">
         <v>374</v>
@@ -1228,7 +1228,7 @@
     </row>
     <row r="16" spans="1:15" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B16" s="16">
         <v>374</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="18" spans="1:10" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="16">
         <v>374</v>

</xml_diff>